<commit_message>
Updated lots of the practice problems--Almost finished with these.
</commit_message>
<xml_diff>
--- a/Schedule/SA405_Schedule_2021.xlsx
+++ b/Schedule/SA405_Schedule_2021.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rcurry/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rcurry/Desktop/SA405/Schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A195917-D83D-9D4B-BDC3-BF0078744C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3740D04-0429-E94A-A273-65C66C6F2EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15920" yWindow="520" windowWidth="21340" windowHeight="16940" xr2:uid="{C4E24355-394D-194D-9B97-FD6EA393468F}"/>
+    <workbookView xWindow="16660" yWindow="520" windowWidth="16940" windowHeight="16940" xr2:uid="{C4E24355-394D-194D-9B97-FD6EA393468F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tuesday_Thursday_Schedule" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="100">
   <si>
     <t>Week</t>
   </si>
@@ -281,13 +281,67 @@
   </si>
   <si>
     <t>Project Paper Due</t>
+  </si>
+  <si>
+    <t>Lesson 1</t>
+  </si>
+  <si>
+    <t>Lesson 2</t>
+  </si>
+  <si>
+    <t>Modeling Review</t>
+  </si>
+  <si>
+    <t>Jupyter Review</t>
+  </si>
+  <si>
+    <t>Network Models</t>
+  </si>
+  <si>
+    <t>Shortest Path</t>
+  </si>
+  <si>
+    <t>Modeling Functions in Jupyter</t>
+  </si>
+  <si>
+    <t>Fixed Charge</t>
+  </si>
+  <si>
+    <t>Set Covering</t>
+  </si>
+  <si>
+    <t>Logical Constraints</t>
+  </si>
+  <si>
+    <t>Python Review</t>
+  </si>
+  <si>
+    <t>Min Spanning Tree</t>
+  </si>
+  <si>
+    <t>TSP</t>
+  </si>
+  <si>
+    <t>VRP</t>
+  </si>
+  <si>
+    <t>Facility Location</t>
+  </si>
+  <si>
+    <t>IP Formulations</t>
+  </si>
+  <si>
+    <t>More IP Formulations</t>
+  </si>
+  <si>
+    <t>Branch &amp; Bound</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -306,6 +360,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -378,19 +438,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -710,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72FE16-6A5A-C340-B26E-F3176A04C1E9}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -769,7 +829,7 @@
       <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>60</v>
       </c>
     </row>
@@ -783,13 +843,13 @@
       <c r="D3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>61</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="7" t="s">
         <v>62</v>
       </c>
     </row>
@@ -800,19 +860,19 @@
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="9" t="s">
         <v>63</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="7" t="s">
         <v>64</v>
       </c>
     </row>
@@ -826,13 +886,13 @@
       <c r="D5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="9" t="s">
         <v>65</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="7" t="s">
         <v>67</v>
       </c>
     </row>
@@ -846,13 +906,13 @@
       <c r="D6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="10" t="s">
         <v>66</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="7" t="s">
         <v>68</v>
       </c>
     </row>
@@ -872,10 +932,10 @@
         <v>29</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="11"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -890,7 +950,7 @@
       <c r="F8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="7" t="s">
         <v>72</v>
       </c>
     </row>
@@ -904,13 +964,13 @@
       <c r="D9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="9" t="s">
         <v>69</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="7" t="s">
         <v>73</v>
       </c>
     </row>
@@ -924,13 +984,13 @@
       <c r="D10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="9" t="s">
         <v>70</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="7" t="s">
         <v>74</v>
       </c>
     </row>
@@ -941,19 +1001,19 @@
       <c r="B11">
         <v>11</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="10" t="s">
         <v>71</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="7" t="s">
         <v>75</v>
       </c>
     </row>
@@ -965,16 +1025,18 @@
         <v>12</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="4"/>
+      <c r="I12" s="11"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -986,10 +1048,10 @@
       <c r="D13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="7" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1003,13 +1065,13 @@
       <c r="D14" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="9" t="s">
         <v>76</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="7" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1026,10 +1088,10 @@
       <c r="E15" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="6"/>
+      <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1041,13 +1103,13 @@
       <c r="D16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="9" t="s">
         <v>79</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="8" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1072,50 +1134,178 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="5">
         <v>18</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="H18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I18" s="8"/>
+      <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="5">
         <v>19</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" t="s">
+        <v>99</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1123,6 +1313,7 @@
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="F15:G15"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>